<commit_message>
Adicionando o caminho certo para o Shared do orch do login T2c
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -238,10 +238,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,7 +540,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>